<commit_message>
Se corrigio como se muestran las fechas en el data grid, falta el instalador
</commit_message>
<xml_diff>
--- a/ncs/Planilla de Elementos.xlsx
+++ b/ncs/Planilla de Elementos.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10">
+<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <x:workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8f9b613cb27ae263/Escritorio/Control de inventario/ncs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9CCC818D-1C78-4F29-8EC3-4B9D8100FD59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{9CCC818D-1C78-4F29-8EC3-4B9D8100FD59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E5A6084-049D-4B0B-A978-2F6E927F007A}"/>
   <x:bookViews>
-    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" tabRatio="410" firstSheet="0" activeTab="0"/>
+    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" tabRatio="410" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -96,7 +96,7 @@
     <x:t>Pp</x:t>
   </x:si>
   <x:si>
-    <x:t>Monitor  Samsung CD6589</x:t>
+    <x:t>Monitor LG 770</x:t>
   </x:si>
   <x:si>
     <x:t/>
@@ -172,20 +172,17 @@
   </x:si>
   <x:si>
     <x:t>Formulario Único</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Producto de prueba </x:t>
   </x:si>
 </x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2">
+<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
   <x:numFmts count="4">
-    <x:numFmt numFmtId="170" formatCode="0000"/>
-    <x:numFmt numFmtId="171" formatCode="000"/>
-    <x:numFmt numFmtId="172" formatCode="[$$-2C0A]#,##0.00;[Red]\([$$-2C0A]#,##0.00\)"/>
-    <x:numFmt numFmtId="173" formatCode="dd/mm/yy"/>
+    <x:numFmt numFmtId="164" formatCode="0000"/>
+    <x:numFmt numFmtId="165" formatCode="000"/>
+    <x:numFmt numFmtId="166" formatCode="[$$-2C0A]#,##0.00;[Red]\([$$-2C0A]#,##0.00\)"/>
+    <x:numFmt numFmtId="167" formatCode="dd/mm/yy"/>
   </x:numFmts>
   <x:fonts count="7" x14ac:knownFonts="1">
     <x:font>
@@ -376,13 +373,13 @@
     <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="170" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="171" fontId="2" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="165" fontId="2" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
@@ -400,7 +397,7 @@
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="172" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="166" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="11" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -409,7 +406,7 @@
     <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="173" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="167" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -446,19 +443,41 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="48">
+  <x:cellXfs count="39">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <x:alignment horizontal="right"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <x:xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <x:alignment horizontal="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <x:alignment horizontal="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <x:alignment horizontal="center" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="right"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <x:alignment horizontal="center"/>
     </x:xf>
-    <x:xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <x:alignment horizontal="center"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <x:alignment horizontal="left"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <x:alignment vertical="center"/>
     </x:xf>
-    <x:xf numFmtId="171" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <x:xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <x:alignment horizontal="left"/>
     </x:xf>
     <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -466,10 +485,6 @@
     </x:xf>
     <x:xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <x:alignment horizontal="center" vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <x:alignment horizontal="left"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <x:alignment horizontal="center" vertical="center"/>
@@ -478,13 +493,10 @@
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <x:alignment horizontal="center"/>
     </x:xf>
-    <x:xf numFmtId="172" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <x:xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <x:alignment horizontal="justify"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <x:alignment horizontal="center"/>
-    </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <x:alignment horizontal="center"/>
     </x:xf>
@@ -496,7 +508,6 @@
     </x:xf>
     <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <x:xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -506,48 +517,11 @@
     <x:xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="left"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="right"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <x:alignment horizontal="center" vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <x:alignment horizontal="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <x:alignment horizontal="right"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <x:alignment horizontal="center"/>
-    </x:xf>
-    <x:xf numFmtId="173" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <x:alignment horizontal="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <x:alignment horizontal="right"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellXfs>
   <x:cellStyles count="1">
@@ -960,15 +934,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
     <x:pageSetUpPr fitToPage="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:P40"/>
+  <x:dimension ref="A1:P34"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <x:selection activeCell="B13" sqref="B13 B13:D13"/>
+      <x:selection activeCell="G10" sqref="G10"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr baseColWidth="10" defaultColWidth="11.424911" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -979,7 +953,7 @@
     <x:col min="4" max="4" width="11.570312" style="0" customWidth="1"/>
     <x:col min="5" max="6" width="6.140625" style="0" customWidth="1"/>
     <x:col min="7" max="7" width="12" style="0" customWidth="1"/>
-    <x:col min="8" max="8" width="11.420625" style="0" customWidth="1"/>
+    <x:col min="8" max="8" width="11.425781" style="0" customWidth="1"/>
     <x:col min="9" max="12" width="4.855469" style="0" customWidth="1"/>
     <x:col min="13" max="13" width="11.140625" style="0" customWidth="1"/>
     <x:col min="14" max="14" width="17.570312" style="0" customWidth="1"/>
@@ -989,567 +963,563 @@
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="D1" s="1" t="s">
+      <x:c r="D1" s="11" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="E1" s="1"/>
-      <x:c r="F1" s="1"/>
-      <x:c r="G1" s="1"/>
-      <x:c r="H1" s="1"/>
-      <x:c r="I1" s="1"/>
-      <x:c r="J1" s="1"/>
-      <x:c r="K1" s="1"/>
-      <x:c r="L1" s="1"/>
+      <x:c r="E1" s="11"/>
+      <x:c r="F1" s="11"/>
+      <x:c r="G1" s="11"/>
+      <x:c r="H1" s="11"/>
+      <x:c r="I1" s="11"/>
+      <x:c r="J1" s="11"/>
+      <x:c r="K1" s="11"/>
+      <x:c r="L1" s="11"/>
       <x:c r="N1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="D2" s="2"/>
-      <x:c r="E2" s="2"/>
-      <x:c r="M2" s="4" t="s">
+      <x:c r="D2" s="13"/>
+      <x:c r="E2" s="13"/>
+      <x:c r="M2" s="14" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="N2" s="5"/>
+      <x:c r="N2" s="15"/>
     </x:row>
     <x:row r="3" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="D3" s="6"/>
-      <x:c r="E3" s="6"/>
-      <x:c r="M3" s="4" t="s">
+      <x:c r="D3" s="16"/>
+      <x:c r="E3" s="16"/>
+      <x:c r="M3" s="14" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="N3" s="7">
+      <x:c r="N3" s="17">
         <x:v>45841</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:16" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="D4" s="6"/>
-      <x:c r="E4" s="6"/>
-      <x:c r="N4" s="6"/>
+      <x:c r="D4" s="16"/>
+      <x:c r="E4" s="16"/>
+      <x:c r="N4" s="16"/>
     </x:row>
     <x:row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <x:c r="A5" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="C5" s="44" t="s">
+      <x:c r="C5" s="10" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="D5" s="44"/>
-      <x:c r="E5" s="44"/>
-      <x:c r="G5" s="45" t="s">
+      <x:c r="D5" s="10"/>
+      <x:c r="E5" s="10"/>
+      <x:c r="G5" s="9" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="H5" s="45"/>
-      <x:c r="I5" s="44" t="s">
+      <x:c r="H5" s="9"/>
+      <x:c r="I5" s="10" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="J5" s="44"/>
-      <x:c r="K5" s="44"/>
-      <x:c r="L5" s="46"/>
-      <x:c r="M5" s="46"/>
-      <x:c r="N5" s="46"/>
+      <x:c r="J5" s="10"/>
+      <x:c r="K5" s="10"/>
+      <x:c r="L5" s="37"/>
+      <x:c r="M5" s="37"/>
+      <x:c r="N5" s="37"/>
     </x:row>
     <x:row r="6" spans="1:16" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <x:row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="A7" s="10" t="s">
+      <x:c r="A7" s="8" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="B7" s="10" t="s">
+      <x:c r="B7" s="8" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="C7" s="10"/>
-      <x:c r="D7" s="10"/>
-      <x:c r="E7" s="10" t="s">
+      <x:c r="C7" s="8"/>
+      <x:c r="D7" s="8"/>
+      <x:c r="E7" s="8" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="F7" s="10" t="s">
+      <x:c r="F7" s="8" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="G7" s="10" t="s">
+      <x:c r="G7" s="8" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="H7" s="10"/>
-      <x:c r="I7" s="10" t="s">
+      <x:c r="H7" s="8"/>
+      <x:c r="I7" s="8" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="J7" s="10"/>
-      <x:c r="K7" s="10" t="s">
+      <x:c r="J7" s="8"/>
+      <x:c r="K7" s="8" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="L7" s="10"/>
-      <x:c r="M7" s="10" t="s">
+      <x:c r="L7" s="8"/>
+      <x:c r="M7" s="8" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="N7" s="10"/>
+      <x:c r="N7" s="8"/>
     </x:row>
     <x:row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="A8" s="10" t="s">
+      <x:c r="A8" s="8" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="B8" s="10"/>
-      <x:c r="C8" s="10"/>
-      <x:c r="D8" s="10"/>
-      <x:c r="E8" s="10"/>
-      <x:c r="F8" s="10" t="s">
+      <x:c r="B8" s="8"/>
+      <x:c r="C8" s="8"/>
+      <x:c r="D8" s="8"/>
+      <x:c r="E8" s="8"/>
+      <x:c r="F8" s="8" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="G8" s="10" t="s">
+      <x:c r="G8" s="8" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="H8" s="10" t="s">
+      <x:c r="H8" s="8" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="I8" s="10" t="s">
+      <x:c r="I8" s="8" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="J8" s="10" t="s">
+      <x:c r="J8" s="8" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="K8" s="10" t="s">
+      <x:c r="K8" s="8" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="L8" s="10" t="s">
+      <x:c r="L8" s="8" t="s">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="M8" s="10"/>
-      <x:c r="N8" s="10"/>
+      <x:c r="M8" s="8"/>
+      <x:c r="N8" s="8"/>
     </x:row>
     <x:row r="9" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="A9" s="11">
+      <x:c r="A9" s="5">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="B9" s="36" t="s">
+      <x:c r="B9" s="7" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="C9" s="36"/>
-      <x:c r="D9" s="36"/>
-      <x:c r="E9" s="12"/>
-      <x:c r="F9" s="12">
+      <x:c r="C9" s="7"/>
+      <x:c r="D9" s="7"/>
+      <x:c r="E9" s="20"/>
+      <x:c r="F9" s="20">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="G9" s="21"/>
+      <x:c r="H9" s="21"/>
+      <x:c r="I9" s="20"/>
+      <x:c r="J9" s="20"/>
+      <x:c r="K9" s="20"/>
+      <x:c r="L9" s="5"/>
+      <x:c r="M9" s="6"/>
+      <x:c r="N9" s="6"/>
+    </x:row>
+    <x:row r="10" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <x:c r="A10" s="5">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B10" s="7" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C10" s="7"/>
+      <x:c r="D10" s="7"/>
+      <x:c r="E10" s="20"/>
+      <x:c r="F10" s="20" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="G10" s="21"/>
+      <x:c r="H10" s="21"/>
+      <x:c r="I10" s="20"/>
+      <x:c r="J10" s="20"/>
+      <x:c r="K10" s="20"/>
+      <x:c r="L10" s="5"/>
+      <x:c r="M10" s="6"/>
+      <x:c r="N10" s="6"/>
+    </x:row>
+    <x:row r="11" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <x:c r="A11" s="5">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="G9" s="13">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="H9" s="13"/>
-      <x:c r="I9" s="12"/>
-      <x:c r="J9" s="12"/>
-      <x:c r="K9" s="12"/>
-      <x:c r="L9" s="11"/>
-      <x:c r="M9" s="37"/>
-      <x:c r="N9" s="37"/>
-    </x:row>
-    <x:row r="10" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="A10" s="11">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="B10" s="36" t="s">
-        <x:v>47</x:v>
-      </x:c>
-      <x:c r="C10" s="36"/>
-      <x:c r="D10" s="36"/>
-      <x:c r="E10" s="12"/>
-      <x:c r="F10" s="12">
+      <x:c r="B11" s="7" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C11" s="7"/>
+      <x:c r="D11" s="7"/>
+      <x:c r="E11" s="20"/>
+      <x:c r="F11" s="20" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="G11" s="21"/>
+      <x:c r="H11" s="21"/>
+      <x:c r="I11" s="20"/>
+      <x:c r="J11" s="20"/>
+      <x:c r="K11" s="20"/>
+      <x:c r="L11" s="5"/>
+      <x:c r="M11" s="6"/>
+      <x:c r="N11" s="6"/>
+    </x:row>
+    <x:row r="12" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <x:c r="A12" s="5">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B12" s="7" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C12" s="7"/>
+      <x:c r="D12" s="7"/>
+      <x:c r="E12" s="20"/>
+      <x:c r="F12" s="20" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="G12" s="21"/>
+      <x:c r="H12" s="21"/>
+      <x:c r="I12" s="20"/>
+      <x:c r="J12" s="20"/>
+      <x:c r="K12" s="20"/>
+      <x:c r="L12" s="5"/>
+      <x:c r="M12" s="6"/>
+      <x:c r="N12" s="6"/>
+      <x:c r="P12" s="22"/>
+    </x:row>
+    <x:row r="13" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <x:c r="A13" s="5">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="G10" s="13">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="H10" s="13"/>
-      <x:c r="I10" s="12"/>
-      <x:c r="J10" s="12"/>
-      <x:c r="K10" s="12"/>
-      <x:c r="L10" s="11"/>
-      <x:c r="M10" s="37"/>
-      <x:c r="N10" s="37"/>
-    </x:row>
-    <x:row r="11" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="A11" s="11">
+      <x:c r="B13" s="7" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C13" s="7"/>
+      <x:c r="D13" s="7"/>
+      <x:c r="E13" s="20"/>
+      <x:c r="F13" s="20" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="G13" s="21"/>
+      <x:c r="H13" s="21"/>
+      <x:c r="I13" s="20"/>
+      <x:c r="J13" s="20"/>
+      <x:c r="K13" s="20"/>
+      <x:c r="L13" s="5"/>
+      <x:c r="M13" s="6"/>
+      <x:c r="N13" s="6"/>
+    </x:row>
+    <x:row r="14" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <x:c r="A14" s="5">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B14" s="7" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C14" s="7"/>
+      <x:c r="D14" s="7"/>
+      <x:c r="E14" s="20"/>
+      <x:c r="F14" s="20" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="G14" s="5"/>
+      <x:c r="H14" s="5"/>
+      <x:c r="I14" s="5"/>
+      <x:c r="J14" s="20"/>
+      <x:c r="K14" s="20"/>
+      <x:c r="L14" s="5"/>
+      <x:c r="M14" s="6"/>
+      <x:c r="N14" s="6"/>
+    </x:row>
+    <x:row r="15" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <x:c r="A15" s="5">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="B15" s="7" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C15" s="7"/>
+      <x:c r="D15" s="7"/>
+      <x:c r="E15" s="20"/>
+      <x:c r="F15" s="20" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="G15" s="5"/>
+      <x:c r="H15" s="5"/>
+      <x:c r="I15" s="5"/>
+      <x:c r="J15" s="20"/>
+      <x:c r="K15" s="20"/>
+      <x:c r="L15" s="5"/>
+      <x:c r="M15" s="6"/>
+      <x:c r="N15" s="6"/>
+    </x:row>
+    <x:row r="16" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <x:c r="A16" s="5">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B16" s="7" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C16" s="7"/>
+      <x:c r="D16" s="7"/>
+      <x:c r="E16" s="20"/>
+      <x:c r="F16" s="20" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="G16" s="5"/>
+      <x:c r="H16" s="5"/>
+      <x:c r="I16" s="5"/>
+      <x:c r="J16" s="20"/>
+      <x:c r="K16" s="5"/>
+      <x:c r="L16" s="5"/>
+      <x:c r="M16" s="6"/>
+      <x:c r="N16" s="6"/>
+    </x:row>
+    <x:row r="17" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <x:c r="A17" s="5">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B17" s="7" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C17" s="7"/>
+      <x:c r="D17" s="7"/>
+      <x:c r="E17" s="20"/>
+      <x:c r="F17" s="20" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="G17" s="5"/>
+      <x:c r="H17" s="5"/>
+      <x:c r="I17" s="5"/>
+      <x:c r="J17" s="20"/>
+      <x:c r="K17" s="5"/>
+      <x:c r="L17" s="5"/>
+      <x:c r="M17" s="6"/>
+      <x:c r="N17" s="6"/>
+    </x:row>
+    <x:row r="18" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <x:c r="A18" s="5">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B18" s="7" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C18" s="7"/>
+      <x:c r="D18" s="7"/>
+      <x:c r="E18" s="5"/>
+      <x:c r="F18" s="5" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="G18" s="5"/>
+      <x:c r="H18" s="5"/>
+      <x:c r="I18" s="5"/>
+      <x:c r="J18" s="5"/>
+      <x:c r="K18" s="5"/>
+      <x:c r="L18" s="5"/>
+      <x:c r="M18" s="5"/>
+      <x:c r="N18" s="5"/>
+    </x:row>
+    <x:row r="19" spans="1:16" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+      <x:c r="C19" s="4"/>
+      <x:c r="D19" s="4"/>
+    </x:row>
+    <x:row r="20" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <x:c r="A20" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B20" s="10"/>
+      <x:c r="C20" s="4"/>
+      <x:c r="D20" s="4"/>
+    </x:row>
+    <x:row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <x:c r="A21" s="8" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="B11" s="36" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="C11" s="36"/>
-      <x:c r="D11" s="36"/>
-      <x:c r="E11" s="12"/>
-      <x:c r="F11" s="12" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="G11" s="13"/>
-      <x:c r="H11" s="13"/>
-      <x:c r="I11" s="12"/>
-      <x:c r="J11" s="12"/>
-      <x:c r="K11" s="12"/>
-      <x:c r="L11" s="11"/>
-      <x:c r="M11" s="37"/>
-      <x:c r="N11" s="37"/>
-    </x:row>
-    <x:row r="12" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="A12" s="11">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="B12" s="36" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="C12" s="36"/>
-      <x:c r="D12" s="36"/>
-      <x:c r="E12" s="12"/>
-      <x:c r="F12" s="12" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="G12" s="13"/>
-      <x:c r="H12" s="13"/>
-      <x:c r="I12" s="12"/>
-      <x:c r="J12" s="12"/>
-      <x:c r="K12" s="12"/>
-      <x:c r="L12" s="11"/>
-      <x:c r="M12" s="37"/>
-      <x:c r="N12" s="37"/>
-      <x:c r="P12" s="14"/>
-    </x:row>
-    <x:row r="13" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="A13" s="11">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="B13" s="36" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="C13" s="36"/>
-      <x:c r="D13" s="36"/>
-      <x:c r="E13" s="12"/>
-      <x:c r="F13" s="12" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="G13" s="13"/>
-      <x:c r="H13" s="13"/>
-      <x:c r="I13" s="12"/>
-      <x:c r="J13" s="12"/>
-      <x:c r="K13" s="12"/>
-      <x:c r="L13" s="11"/>
-      <x:c r="M13" s="37"/>
-      <x:c r="N13" s="37"/>
-    </x:row>
-    <x:row r="14" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="A14" s="11">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="B14" s="36" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="C14" s="36"/>
-      <x:c r="D14" s="36"/>
-      <x:c r="E14" s="12"/>
-      <x:c r="F14" s="12" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="G14" s="11"/>
-      <x:c r="H14" s="11"/>
-      <x:c r="I14" s="11"/>
-      <x:c r="J14" s="12"/>
-      <x:c r="K14" s="12"/>
-      <x:c r="L14" s="11"/>
-      <x:c r="M14" s="37"/>
-      <x:c r="N14" s="37"/>
-    </x:row>
-    <x:row r="15" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="A15" s="11">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="B15" s="36" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="C15" s="36"/>
-      <x:c r="D15" s="36"/>
-      <x:c r="E15" s="12"/>
-      <x:c r="F15" s="12" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="G15" s="11"/>
-      <x:c r="H15" s="11"/>
-      <x:c r="I15" s="11"/>
-      <x:c r="J15" s="12"/>
-      <x:c r="K15" s="12"/>
-      <x:c r="L15" s="11"/>
-      <x:c r="M15" s="37"/>
-      <x:c r="N15" s="37"/>
-    </x:row>
-    <x:row r="16" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="A16" s="11">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="B16" s="36" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="C16" s="36"/>
-      <x:c r="D16" s="36"/>
-      <x:c r="E16" s="12"/>
-      <x:c r="F16" s="12" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="G16" s="11"/>
-      <x:c r="H16" s="11"/>
-      <x:c r="I16" s="11"/>
-      <x:c r="J16" s="12"/>
-      <x:c r="K16" s="11"/>
-      <x:c r="L16" s="11"/>
-      <x:c r="M16" s="37"/>
-      <x:c r="N16" s="37"/>
-    </x:row>
-    <x:row r="17" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="A17" s="11">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="B17" s="36" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="C17" s="36"/>
-      <x:c r="D17" s="36"/>
-      <x:c r="E17" s="12"/>
-      <x:c r="F17" s="12" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="G17" s="11"/>
-      <x:c r="H17" s="11"/>
-      <x:c r="I17" s="11"/>
-      <x:c r="J17" s="12"/>
-      <x:c r="K17" s="11"/>
-      <x:c r="L17" s="11"/>
-      <x:c r="M17" s="37"/>
-      <x:c r="N17" s="37"/>
-    </x:row>
-    <x:row r="18" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="A18" s="11">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="B18" s="36" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="C18" s="36"/>
-      <x:c r="D18" s="36"/>
-      <x:c r="E18" s="11"/>
-      <x:c r="F18" s="11" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="G18" s="11"/>
-      <x:c r="H18" s="11"/>
-      <x:c r="I18" s="11"/>
-      <x:c r="J18" s="11"/>
-      <x:c r="K18" s="11"/>
-      <x:c r="L18" s="11"/>
-      <x:c r="M18" s="11"/>
-      <x:c r="N18" s="11"/>
-    </x:row>
-    <x:row r="19" spans="1:16" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="C19" s="16"/>
-      <x:c r="D19" s="16"/>
-    </x:row>
-    <x:row r="20" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="A20" s="44" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="B20" s="44"/>
-      <x:c r="C20" s="16"/>
-      <x:c r="D20" s="16"/>
-    </x:row>
-    <x:row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="A21" s="10" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="B21" s="10"/>
-      <x:c r="C21" s="10" t="s">
+      <x:c r="B21" s="8"/>
+      <x:c r="C21" s="8" t="s">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="D21" s="10" t="s">
+      <x:c r="D21" s="8" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="E21" s="10"/>
-      <x:c r="F21" s="10"/>
-      <x:c r="G21" s="10"/>
-      <x:c r="H21" s="10"/>
-      <x:c r="I21" s="10"/>
-      <x:c r="J21" s="10"/>
-      <x:c r="K21" s="10"/>
-      <x:c r="L21" s="10"/>
-      <x:c r="M21" s="10" t="s">
+      <x:c r="E21" s="8"/>
+      <x:c r="F21" s="8"/>
+      <x:c r="G21" s="8"/>
+      <x:c r="H21" s="8"/>
+      <x:c r="I21" s="8"/>
+      <x:c r="J21" s="8"/>
+      <x:c r="K21" s="8"/>
+      <x:c r="L21" s="8"/>
+      <x:c r="M21" s="8" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="N21" s="10"/>
+      <x:c r="N21" s="8"/>
     </x:row>
     <x:row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="A22" s="10"/>
-      <x:c r="B22" s="10"/>
-      <x:c r="C22" s="10" t="s">
+      <x:c r="A22" s="8"/>
+      <x:c r="B22" s="8"/>
+      <x:c r="C22" s="8" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="D22" s="10" t="s">
+      <x:c r="D22" s="8" t="s">
         <x:v>28</x:v>
       </x:c>
-      <x:c r="E22" s="10"/>
-      <x:c r="F22" s="10"/>
-      <x:c r="G22" s="10"/>
-      <x:c r="H22" s="10"/>
-      <x:c r="I22" s="10" t="s">
+      <x:c r="E22" s="8"/>
+      <x:c r="F22" s="8"/>
+      <x:c r="G22" s="8"/>
+      <x:c r="H22" s="8"/>
+      <x:c r="I22" s="8" t="s">
         <x:v>29</x:v>
       </x:c>
-      <x:c r="J22" s="10"/>
-      <x:c r="K22" s="10"/>
-      <x:c r="L22" s="10"/>
-      <x:c r="M22" s="10"/>
-      <x:c r="N22" s="10"/>
+      <x:c r="J22" s="8"/>
+      <x:c r="K22" s="8"/>
+      <x:c r="L22" s="8"/>
+      <x:c r="M22" s="8"/>
+      <x:c r="N22" s="8"/>
     </x:row>
     <x:row r="23" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="A23" s="40"/>
-      <x:c r="B23" s="40"/>
-      <x:c r="C23" s="17"/>
-      <x:c r="D23" s="36"/>
-      <x:c r="E23" s="36"/>
-      <x:c r="F23" s="36"/>
-      <x:c r="G23" s="36"/>
-      <x:c r="H23" s="36"/>
-      <x:c r="I23" s="11"/>
-      <x:c r="J23" s="11"/>
-      <x:c r="K23" s="11"/>
-      <x:c r="L23" s="11"/>
-      <x:c r="M23" s="11"/>
-      <x:c r="N23" s="11"/>
+      <x:c r="A23" s="3"/>
+      <x:c r="B23" s="3"/>
+      <x:c r="C23" s="24"/>
+      <x:c r="D23" s="7"/>
+      <x:c r="E23" s="7"/>
+      <x:c r="F23" s="7"/>
+      <x:c r="G23" s="7"/>
+      <x:c r="H23" s="7"/>
+      <x:c r="I23" s="5"/>
+      <x:c r="J23" s="5"/>
+      <x:c r="K23" s="5"/>
+      <x:c r="L23" s="5"/>
+      <x:c r="M23" s="5"/>
+      <x:c r="N23" s="5"/>
     </x:row>
     <x:row r="24" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="A24" s="11"/>
-      <x:c r="B24" s="11"/>
-      <x:c r="C24" s="11"/>
-      <x:c r="D24" s="11"/>
-      <x:c r="E24" s="11"/>
-      <x:c r="F24" s="11"/>
-      <x:c r="G24" s="11"/>
-      <x:c r="H24" s="11"/>
-      <x:c r="I24" s="11"/>
-      <x:c r="J24" s="11"/>
-      <x:c r="K24" s="11"/>
-      <x:c r="L24" s="11"/>
-      <x:c r="M24" s="11"/>
-      <x:c r="N24" s="11"/>
+      <x:c r="A24" s="5"/>
+      <x:c r="B24" s="5"/>
+      <x:c r="C24" s="5"/>
+      <x:c r="D24" s="5"/>
+      <x:c r="E24" s="5"/>
+      <x:c r="F24" s="5"/>
+      <x:c r="G24" s="5"/>
+      <x:c r="H24" s="5"/>
+      <x:c r="I24" s="5"/>
+      <x:c r="J24" s="5"/>
+      <x:c r="K24" s="5"/>
+      <x:c r="L24" s="5"/>
+      <x:c r="M24" s="5"/>
+      <x:c r="N24" s="5"/>
     </x:row>
     <x:row r="25" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="A25" s="11"/>
-      <x:c r="B25" s="11"/>
-      <x:c r="C25" s="11"/>
-      <x:c r="D25" s="11"/>
-      <x:c r="E25" s="11"/>
-      <x:c r="F25" s="11"/>
-      <x:c r="G25" s="11"/>
-      <x:c r="H25" s="11"/>
-      <x:c r="I25" s="11"/>
-      <x:c r="J25" s="11"/>
-      <x:c r="K25" s="11"/>
-      <x:c r="L25" s="11"/>
-      <x:c r="M25" s="11"/>
-      <x:c r="N25" s="11"/>
+      <x:c r="A25" s="5"/>
+      <x:c r="B25" s="5"/>
+      <x:c r="C25" s="5"/>
+      <x:c r="D25" s="5"/>
+      <x:c r="E25" s="5"/>
+      <x:c r="F25" s="5"/>
+      <x:c r="G25" s="5"/>
+      <x:c r="H25" s="5"/>
+      <x:c r="I25" s="5"/>
+      <x:c r="J25" s="5"/>
+      <x:c r="K25" s="5"/>
+      <x:c r="L25" s="5"/>
+      <x:c r="M25" s="5"/>
+      <x:c r="N25" s="5"/>
     </x:row>
     <x:row r="26" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="A26" s="11"/>
-      <x:c r="B26" s="11"/>
-      <x:c r="C26" s="11"/>
-      <x:c r="D26" s="11"/>
-      <x:c r="E26" s="11"/>
-      <x:c r="F26" s="11"/>
-      <x:c r="G26" s="11"/>
-      <x:c r="H26" s="11"/>
-      <x:c r="I26" s="11"/>
-      <x:c r="J26" s="11"/>
-      <x:c r="K26" s="11"/>
-      <x:c r="L26" s="11"/>
-      <x:c r="M26" s="11"/>
-      <x:c r="N26" s="11"/>
+      <x:c r="A26" s="5"/>
+      <x:c r="B26" s="5"/>
+      <x:c r="C26" s="5"/>
+      <x:c r="D26" s="5"/>
+      <x:c r="E26" s="5"/>
+      <x:c r="F26" s="5"/>
+      <x:c r="G26" s="5"/>
+      <x:c r="H26" s="5"/>
+      <x:c r="I26" s="5"/>
+      <x:c r="J26" s="5"/>
+      <x:c r="K26" s="5"/>
+      <x:c r="L26" s="5"/>
+      <x:c r="M26" s="5"/>
+      <x:c r="N26" s="5"/>
     </x:row>
     <x:row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="M27" s="43"/>
-      <x:c r="N27" s="43"/>
-    </x:row>
-    <x:row r="28" spans="1:16" ht="15.75" customHeight="1" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <x:c r="A28" s="18" t="s">
+      <x:c r="M27" s="1"/>
+      <x:c r="N27" s="1"/>
+    </x:row>
+    <x:row r="28" spans="1:16" ht="15.75" customHeight="1" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <x:c r="A28" s="25" t="s">
         <x:v>30</x:v>
       </x:c>
-      <x:c r="G28" s="19" t="s">
+      <x:c r="G28" s="26" t="s">
         <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="A29" s="20" t="s">
+      <x:c r="A29" s="27" t="s">
         <x:v>32</x:v>
       </x:c>
-      <x:c r="B29" s="19" t="s">
+      <x:c r="B29" s="26" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="C29" s="19"/>
-      <x:c r="I29" s="22"/>
-      <x:c r="J29" s="23"/>
-      <x:c r="K29" s="23"/>
-      <x:c r="L29" s="23"/>
-      <x:c r="M29" s="23"/>
-      <x:c r="N29" s="24"/>
+      <x:c r="C29" s="26"/>
+      <x:c r="I29" s="28"/>
+      <x:c r="J29" s="29"/>
+      <x:c r="K29" s="29"/>
+      <x:c r="L29" s="29"/>
+      <x:c r="M29" s="29"/>
+      <x:c r="N29" s="30"/>
     </x:row>
     <x:row r="30" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="A30" s="20" t="s">
+      <x:c r="A30" s="27" t="s">
         <x:v>34</x:v>
       </x:c>
-      <x:c r="B30" s="19" t="s">
+      <x:c r="B30" s="26" t="s">
         <x:v>35</x:v>
       </x:c>
-      <x:c r="C30" s="19"/>
-      <x:c r="I30" s="25"/>
-      <x:c r="N30" s="26"/>
+      <x:c r="C30" s="26"/>
+      <x:c r="I30" s="31"/>
+      <x:c r="N30" s="32"/>
     </x:row>
     <x:row r="31" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="A31" s="20" t="s">
+      <x:c r="A31" s="27" t="s">
         <x:v>36</x:v>
       </x:c>
-      <x:c r="B31" s="19" t="s">
+      <x:c r="B31" s="26" t="s">
         <x:v>37</x:v>
       </x:c>
-      <x:c r="C31" s="19"/>
-      <x:c r="I31" s="25"/>
-      <x:c r="N31" s="26"/>
+      <x:c r="C31" s="26"/>
+      <x:c r="I31" s="31"/>
+      <x:c r="N31" s="32"/>
     </x:row>
     <x:row r="32" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="A32" s="20" t="s">
+      <x:c r="A32" s="27" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="B32" s="19" t="s">
+      <x:c r="B32" s="26" t="s">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="C32" s="19"/>
-      <x:c r="I32" s="27" t="s">
+      <x:c r="C32" s="26"/>
+      <x:c r="I32" s="33" t="s">
         <x:v>40</x:v>
       </x:c>
-      <x:c r="J32" s="28"/>
-      <x:c r="K32" s="29"/>
-      <x:c r="L32" s="29"/>
-      <x:c r="M32" s="29" t="s">
+      <x:c r="J32" s="34"/>
+      <x:c r="K32" s="35"/>
+      <x:c r="L32" s="35"/>
+      <x:c r="M32" s="35" t="s">
         <x:v>41</x:v>
       </x:c>
-      <x:c r="N32" s="30"/>
+      <x:c r="N32" s="36"/>
     </x:row>
     <x:row r="33" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="A33" s="20" t="s">
+      <x:c r="A33" s="27" t="s">
         <x:v>42</x:v>
       </x:c>
-      <x:c r="B33" s="19" t="s">
+      <x:c r="B33" s="26" t="s">
         <x:v>43</x:v>
       </x:c>
-      <x:c r="C33" s="19"/>
+      <x:c r="C33" s="26"/>
     </x:row>
     <x:row r="34" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="A34" s="20" t="s">
+      <x:c r="A34" s="27" t="s">
         <x:v>44</x:v>
       </x:c>
-      <x:c r="B34" s="19" t="s">
+      <x:c r="B34" s="26" t="s">
         <x:v>45</x:v>
       </x:c>
-      <x:c r="C34" s="19"/>
-      <x:c r="N34" s="47" t="s">
+      <x:c r="C34" s="26"/>
+      <x:c r="N34" s="38" t="s">
         <x:v>46</x:v>
       </x:c>
-      <x:c r="O34" s="47"/>
+      <x:c r="O34" s="38"/>
     </x:row>
   </x:sheetData>
   <x:mergeCells count="60">
@@ -1625,7 +1595,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0100-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
@@ -1645,7 +1615,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0200-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>

</xml_diff>